<commit_message>
Actualizadas actividades y lecturas semana 3
</commit_message>
<xml_diff>
--- a/Actividades/IntervalosConfianzaT.xlsx
+++ b/Actividades/IntervalosConfianzaT.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="19560" windowHeight="8205" activeTab="2"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="19560" windowHeight="8205" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -111,7 +111,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -186,7 +186,7 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
@@ -2337,7 +2337,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D19" sqref="D19:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>